<commit_message>
ng: update Kwara forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Nigeria/2024/oct_2024/Kwara/ng_lf_tas_2410_1_sit_part_kw.xlsx
+++ b/LF/TAS/Nigeria/2024/oct_2024/Kwara/ng_lf_tas_2410_1_sit_part_kw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Nigeria\2024\oct_2024\Kwara\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F3AADC-ACB6-4D76-9BA7-5E30BFAB7C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED6374F-BB75-4366-9301-123D6BEBCFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2336,16 +2336,16 @@
     <t>community = ${c_community}</t>
   </si>
   <si>
-    <t>ng_lf_tas_2410_1_sit_part_kw</t>
-  </si>
-  <si>
-    <t>(Octobre 2024) kwara - 1. TAS1 LF Site &amp; participant Form</t>
-  </si>
-  <si>
     <t>KIKPARISONE</t>
   </si>
   <si>
-    <t>ng_tas_p_2410_kw</t>
+    <t>(Octobre 2024) kwara - 1. TAS1 LF Site &amp; participant Form V2</t>
+  </si>
+  <si>
+    <t>ng_lf_tas_2410_1_sit_part_kw_v2</t>
+  </si>
+  <si>
+    <t>ng_tas_p_2410_kw2</t>
   </si>
 </sst>
 </file>
@@ -2643,57 +2643,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3021,7 +2971,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5175,10 +5125,10 @@
         <v>760</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>734</v>
@@ -10953,7 +10903,7 @@
         <v>247</v>
       </c>
       <c r="F522" s="3" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="523" spans="1:6">
@@ -13151,7 +13101,7 @@
         <v>761</v>
       </c>
       <c r="F679" s="3" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="680" spans="1:6">
@@ -20782,7 +20732,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -20812,7 +20762,7 @@
         <v>767</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>51</v>
@@ -21856,7 +21806,7 @@
         <v>734</v>
       </c>
       <c r="O28" s="30" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="Q28" s="30" t="s">
         <v>715</v>
@@ -22083,7 +22033,7 @@
         <v>734</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D35" s="30" t="s">
         <v>247</v>
@@ -27074,7 +27024,7 @@
         <v>644</v>
       </c>
       <c r="Q177" s="30" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="R177" s="30" t="s">
         <v>247</v>

</xml_diff>